<commit_message>
Data provider for @Before test annotation created amazon testcase Created Custom annotations with enums
</commit_message>
<xml_diff>
--- a/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
+++ b/SeleniumAutomationProject/src/test/resources/ExcelFiles/TestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
   <si>
     <t>testname</t>
   </si>
@@ -38,27 +38,36 @@
     <t>To check wheather user can successfully Login and logout</t>
   </si>
   <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>newTest1</t>
+  </si>
+  <si>
+    <t>To check wheather test is executed</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>loginLogoutTest2</t>
+  </si>
+  <si>
+    <t>Login logout test 2</t>
+  </si>
+  <si>
+    <t>amazonTest</t>
+  </si>
+  <si>
+    <t>Demo checking with other sites</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>newTest1</t>
-  </si>
-  <si>
-    <t>To check wheather test is executed</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>loginLogoutTest2</t>
-  </si>
-  <si>
-    <t>Login logout test 2</t>
-  </si>
-  <si>
     <t>browser</t>
   </si>
   <si>
@@ -71,6 +80,9 @@
     <t>faname</t>
   </si>
   <si>
+    <t>items</t>
+  </si>
+  <si>
     <t>chrome</t>
   </si>
   <si>
@@ -83,25 +95,31 @@
     <t>vasanth</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>firefox</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>admin1234</t>
   </si>
   <si>
     <t>malathi</t>
   </si>
   <si>
-    <t>no</t>
-  </si>
-  <si>
     <t>edge</t>
   </si>
   <si>
     <t>pavan</t>
+  </si>
+  <si>
+    <t>Mobiles, Computers</t>
+  </si>
+  <si>
+    <t>TV, Appliances, Electronics</t>
+  </si>
+  <si>
+    <t>Women's Fashion</t>
   </si>
 </sst>
 </file>
@@ -114,13 +132,19 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -587,144 +611,150 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1046,13 +1076,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="20.8181818181818" customWidth="1"/>
     <col min="2" max="2" width="52.5454545454545" customWidth="1"/>
@@ -1085,7 +1115,7 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -1102,10 +1132,10 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1119,10 +1149,27 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1135,21 +1182,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="21.1818181818182" customWidth="1"/>
     <col min="2" max="4" width="10.3636363636364" customWidth="1"/>
     <col min="5" max="5" width="14.8181818181818" customWidth="1"/>
     <col min="6" max="6" width="12.2727272727273" customWidth="1"/>
+    <col min="7" max="7" width="24.6363636363636" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1157,116 +1205,203 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>28</v>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>